<commit_message>
alterando conforme passagem para zurique
</commit_message>
<xml_diff>
--- a/despesas.xlsx
+++ b/despesas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camilat2003_00\Desktop\Pessoais\Europa 06-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7F74CA-0640-4390-BBDF-F8D6140764FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36F2B51-366D-42ED-8ED4-2551BBF9A6B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Data</t>
   </si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t>Coluna2</t>
+  </si>
+  <si>
+    <t>1250 reais (G-S)</t>
+  </si>
+  <si>
+    <t>Avião da Grécia para Suiça</t>
   </si>
 </sst>
 </file>
@@ -534,7 +540,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -585,10 +591,6 @@
     <xf numFmtId="0" fontId="10" fillId="9" borderId="12" xfId="8" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
       <protection locked="0"/>
@@ -615,6 +617,13 @@
     </xf>
     <xf numFmtId="4" fontId="7" fillId="0" borderId="12" xfId="6" applyBorder="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="5" xfId="12" applyFont="1" applyBorder="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -643,10 +652,10 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.39997558519241921"/>
+          <bgColor theme="6" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color theme="4" tint="-0.249977111117893"/>
         </left>
@@ -655,100 +664,6 @@
         </right>
         <top/>
         <bottom/>
-        <vertical style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </right>
-        <top style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </right>
-        <top style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </right>
-        <top style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </right>
-        <top style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -792,21 +707,25 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color theme="4" tint="-0.249977111117893"/>
         </left>
         <right style="thin">
           <color theme="4" tint="-0.249977111117893"/>
         </right>
-        <top/>
-        <bottom/>
+        <top style="thin">
+          <color theme="4" tint="-0.249977111117893"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="-0.249977111117893"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="4" tint="-0.249977111117893"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="4" tint="-0.249977111117893"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -826,6 +745,28 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="-0.249977111117893"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="-0.249977111117893"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="-0.249977111117893"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="-0.249977111117893"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="4" tint="-0.249977111117893"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="4" tint="-0.249977111117893"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -840,6 +781,28 @@
         <bottom/>
       </border>
       <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="-0.249977111117893"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="-0.249977111117893"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="-0.249977111117893"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="-0.249977111117893"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="4" tint="-0.249977111117893"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="4" tint="-0.249977111117893"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -874,6 +837,28 @@
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="-0.249977111117893"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="-0.249977111117893"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="-0.249977111117893"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="-0.249977111117893"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="4" tint="-0.249977111117893"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="4" tint="-0.249977111117893"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -898,6 +883,22 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="-0.249977111117893"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="-0.249977111117893"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="-0.249977111117893"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="-0.249977111117893"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color theme="4" tint="-0.249977111117893"/>
@@ -905,6 +906,12 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color theme="4" tint="-0.249977111117893"/>
@@ -912,12 +919,14 @@
         <right style="thin">
           <color theme="4" tint="-0.249977111117893"/>
         </right>
-        <top style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </bottom>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color theme="4" tint="-0.249977111117893"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="4" tint="-0.249977111117893"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -998,14 +1007,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9CBFAF6A-671A-4327-A234-291691FC8518}" name="Despesas34" displayName="Despesas34" ref="A2:E9" totalsRowCount="1" headerRowDxfId="0" totalsRowDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9CBFAF6A-671A-4327-A234-291691FC8518}" name="Despesas34" displayName="Despesas34" ref="A2:E9" totalsRowCount="1" headerRowDxfId="13" totalsRowDxfId="10" headerRowBorderDxfId="12" tableBorderDxfId="11">
   <autoFilter ref="A2:E8" xr:uid="{9CBFAF6A-671A-4327-A234-291691FC8518}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{BE5774F8-3D3B-4BD6-AE94-1FF1AC4D65AC}" name="Data" totalsRowLabel="Total" dataDxfId="5" totalsRowDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{0A16F98A-F7D1-4252-B11B-E033E70EA158}" name="Descrição da Despesa" dataDxfId="4" totalsRowDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{EE168068-1FA4-4934-B3F9-78C2616A50BF}" name="Valor" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{F95EA42B-7C3F-4C15-A5D0-2009982AE3F7}" name="Coluna1" dataDxfId="2" totalsRowDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{09FA7907-E59F-4EE8-A7BB-00CDDBCBF60D}" name="Coluna2" dataDxfId="1" totalsRowDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{BE5774F8-3D3B-4BD6-AE94-1FF1AC4D65AC}" name="Data" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{0A16F98A-F7D1-4252-B11B-E033E70EA158}" name="Descrição da Despesa" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{EE168068-1FA4-4934-B3F9-78C2616A50BF}" name="Valor" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{F95EA42B-7C3F-4C15-A5D0-2009982AE3F7}" name="Coluna1" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{09FA7907-E59F-4EE8-A7BB-00CDDBCBF60D}" name="Coluna2" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Relatório de despesas de viagem" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1245,17 +1254,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AAE77B6-366C-4730-A58A-C0C13BE3675F}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="90.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="78.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5" style="3" customWidth="1"/>
-    <col min="2" max="2" width="26.5" style="2" customWidth="1"/>
-    <col min="3" max="4" width="11" style="2" customWidth="1"/>
-    <col min="5" max="5" width="7.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.625" customWidth="1"/>
+    <col min="1" max="1" width="5.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.75" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.875" bestFit="1" customWidth="1"/>
@@ -1276,6 +1285,23 @@
       </c>
       <c r="E1" s="4" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="24">
+        <v>1250</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1354,26 +1380,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D50BE8B2-990A-4D87-83F2-E814EEC1B90B}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="32.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
@@ -1385,106 +1412,108 @@
       <c r="C2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="21" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="23">
+      <c r="A3" s="22">
         <f ca="1">TODAY()-30</f>
-        <v>45138</v>
-      </c>
-      <c r="B3" s="19" t="s">
+        <v>45139</v>
+      </c>
+      <c r="B3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="24">
+      <c r="C3" s="23">
         <v>10000</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="23">
+      <c r="A4" s="22">
         <f ca="1">TODAY()-30</f>
-        <v>45138</v>
-      </c>
-      <c r="B4" s="19" t="s">
+        <v>45139</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="23">
         <v>3015</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="23">
+      <c r="A5" s="22">
         <f ca="1">TODAY()-30</f>
-        <v>45138</v>
-      </c>
-      <c r="B5" s="19" t="s">
+        <v>45139</v>
+      </c>
+      <c r="B5" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="23">
         <v>7800</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="19" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="23">
+      <c r="A6" s="22">
         <f t="shared" ref="A6:A7" ca="1" si="0">TODAY()-30</f>
-        <v>45138</v>
-      </c>
-      <c r="B6" s="19" t="s">
+        <v>45139</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="23">
+      <c r="A7" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>45138</v>
-      </c>
-      <c r="B7" s="19" t="s">
+        <v>45139</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="23">
+      <c r="A8" s="22">
         <f ca="1">TODAY()-25</f>
-        <v>45143</v>
-      </c>
-      <c r="B8" s="19" t="s">
+        <v>45144</v>
+      </c>
+      <c r="B8" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="13"/>
-      <c r="C9" s="18">
+      <c r="C9" s="17">
         <f>SUBTOTAL(109,Despesas34[Valor])</f>
         <v>20815</v>
       </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">

</xml_diff>

<commit_message>
colocando o h em z
</commit_message>
<xml_diff>
--- a/despesas.xlsx
+++ b/despesas.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camilat2003_00\Desktop\Pessoais\Europa 06-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36F2B51-366D-42ED-8ED4-2551BBF9A6B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7F6E9E-F592-46D1-B195-1E4E0607148F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="2" r:id="rId1"/>
     <sheet name="Planilha2" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$E$2</definedName>
     <definedName name="TaxaDeQuilometragem">#REF!</definedName>
     <definedName name="TítuloColuna1">#REF!</definedName>
     <definedName name="TotalDoReembolso">#REF!</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>Data</t>
   </si>
@@ -141,6 +142,9 @@
   </si>
   <si>
     <t>Avião da Grécia para Suiça</t>
+  </si>
+  <si>
+    <t>Hotel</t>
   </si>
 </sst>
 </file>
@@ -152,7 +156,7 @@
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="2" tint="-0.89996032593768116"/>
@@ -265,8 +269,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -321,12 +333,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
+        <fgColor theme="3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -390,21 +408,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color theme="3"/>
       </left>
       <right/>
@@ -469,27 +472,127 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="4" tint="-0.249977111117893"/>
+        <color theme="7"/>
       </left>
       <right style="thin">
-        <color theme="4" tint="-0.249977111117893"/>
+        <color theme="7"/>
       </right>
       <top style="thin">
-        <color theme="4" tint="-0.249977111117893"/>
+        <color theme="7"/>
       </top>
       <bottom style="thin">
-        <color theme="4" tint="-0.249977111117893"/>
+        <color theme="7"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color theme="4" tint="-0.249977111117893"/>
+        <color theme="4" tint="0.59999389629810485"/>
       </left>
       <right style="thin">
-        <color theme="4" tint="-0.249977111117893"/>
+        <color theme="4" tint="0.59999389629810485"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.59999389629810485"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.59999389629810485"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.59999389629810485"/>
       </right>
       <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.59999389629810485"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.59999389629810485"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="0.59999389629810485"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.59999389629810485"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.59999389629810485"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.59999389629810485"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.59999389629810485"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.59999389629810485"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.59999389629810485"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.59999389629810485"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.59999389629810485"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.59999389629810485"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.59999389629810485"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.59999389629810485"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.59999389629810485"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="0.59999389629810485"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.59999389629810485"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.59999389629810485"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.59999389629810485"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -540,7 +643,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -550,76 +653,91 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="11" xfId="12" applyFont="1" applyBorder="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="12" xfId="8" applyFill="1" applyBorder="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="13" xfId="8" applyFill="1" applyBorder="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="12" xfId="8" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="14" xfId="8" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="16" xfId="15" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="12" xfId="15" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="4" fontId="7" fillId="0" borderId="12" xfId="6" applyBorder="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="7" fontId="0" fillId="0" borderId="5" xfId="12" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="11" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="7" xfId="12" applyFont="1" applyBorder="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -647,162 +765,152 @@
     <cellStyle name="Título 4" xfId="14" builtinId="19" hidden="1" customBuiltin="1"/>
     <cellStyle name="Total" xfId="3" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="18">
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.39997558519241921"/>
+          <bgColor theme="4" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
+          <color theme="4" tint="0.59999389629810485"/>
         </left>
-        <right style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </right>
-        <top/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </top>
         <bottom/>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </right>
-        <top style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.39997558519241921"/>
+          <bgColor theme="4" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
+          <color theme="4" tint="0.59999389629810485"/>
         </left>
         <right style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
+          <color theme="4" tint="0.59999389629810485"/>
         </right>
-        <top/>
+        <top style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </top>
         <bottom/>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </right>
-        <top style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="4" formatCode="#,##0.00"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.39997558519241921"/>
+          <bgColor theme="4" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
+        <left style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </top>
         <bottom/>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </right>
-        <top style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.39997558519241921"/>
+          <bgColor theme="4" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
+        <left style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </top>
         <bottom/>
       </border>
       <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </right>
-        <top style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </horizontal>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -816,7 +924,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color theme="1"/>
+        <color theme="0"/>
         <name val="Calibri Light"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -824,14 +932,18 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.39997558519241921"/>
+          <bgColor theme="4" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
-        <right/>
-        <top/>
+        <right style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </top>
         <bottom/>
       </border>
       <protection locked="0" hidden="0"/>
@@ -839,69 +951,172 @@
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
+          <color theme="4" tint="0.59999389629810485"/>
         </left>
-        <right style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </right>
+        <right/>
         <top style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
+          <color theme="4" tint="0.59999389629810485"/>
         </top>
         <bottom style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
+          <color theme="4" tint="0.59999389629810485"/>
         </bottom>
         <vertical style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
+          <color theme="4" tint="0.59999389629810485"/>
         </vertical>
         <horizontal style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
+          <color theme="4" tint="0.59999389629810485"/>
         </horizontal>
       </border>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
+          <color theme="4" tint="0.59999389629810485"/>
         </left>
         <right style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
+          <color theme="4" tint="0.59999389629810485"/>
         </right>
         <top style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
+          <color theme="4" tint="0.59999389629810485"/>
         </top>
         <bottom style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
+          <color theme="4" tint="0.59999389629810485"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.59999389629810485"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
       <border>
         <bottom style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
+          <color theme="4" tint="0.59999389629810485"/>
         </bottom>
       </border>
     </dxf>
@@ -914,18 +1129,18 @@
       </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
+          <color theme="4" tint="0.59999389629810485"/>
         </left>
         <right style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
+          <color theme="4" tint="0.59999389629810485"/>
         </right>
         <top/>
         <bottom/>
         <vertical style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
+          <color theme="4" tint="0.59999389629810485"/>
         </vertical>
         <horizontal style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
+          <color theme="4" tint="0.59999389629810485"/>
         </horizontal>
       </border>
     </dxf>
@@ -990,9 +1205,9 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Relatório de despesas de viagem" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Relatório de despesas de viagem" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="16"/>
-      <tableStyleElement type="headerRow" dxfId="15"/>
-      <tableStyleElement type="totalRow" dxfId="14"/>
+      <tableStyleElement type="wholeTable" dxfId="17"/>
+      <tableStyleElement type="headerRow" dxfId="16"/>
+      <tableStyleElement type="totalRow" dxfId="15"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1007,14 +1222,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9CBFAF6A-671A-4327-A234-291691FC8518}" name="Despesas34" displayName="Despesas34" ref="A2:E9" totalsRowCount="1" headerRowDxfId="13" totalsRowDxfId="10" headerRowBorderDxfId="12" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9CBFAF6A-671A-4327-A234-291691FC8518}" name="Despesas34" displayName="Despesas34" ref="A2:E9" totalsRowCount="1" headerRowDxfId="14" totalsRowDxfId="11" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="10">
   <autoFilter ref="A2:E8" xr:uid="{9CBFAF6A-671A-4327-A234-291691FC8518}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{BE5774F8-3D3B-4BD6-AE94-1FF1AC4D65AC}" name="Data" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{0A16F98A-F7D1-4252-B11B-E033E70EA158}" name="Descrição da Despesa" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{EE168068-1FA4-4934-B3F9-78C2616A50BF}" name="Valor" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{F95EA42B-7C3F-4C15-A5D0-2009982AE3F7}" name="Coluna1" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{09FA7907-E59F-4EE8-A7BB-00CDDBCBF60D}" name="Coluna2" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{BE5774F8-3D3B-4BD6-AE94-1FF1AC4D65AC}" name="Data" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{0A16F98A-F7D1-4252-B11B-E033E70EA158}" name="Descrição da Despesa" dataDxfId="8" totalsRowDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{EE168068-1FA4-4934-B3F9-78C2616A50BF}" name="Valor" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{F95EA42B-7C3F-4C15-A5D0-2009982AE3F7}" name="Coluna1" dataDxfId="6" totalsRowDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{09FA7907-E59F-4EE8-A7BB-00CDDBCBF60D}" name="Coluna2" dataDxfId="5" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Relatório de despesas de viagem" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1252,115 +1467,176 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AAE77B6-366C-4730-A58A-C0C13BE3675F}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="78.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="111.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.75" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="19.625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="11" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="24">
+      <c r="E2" s="14">
         <v>1250</v>
       </c>
     </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="14">
+        <v>3083</v>
+      </c>
+    </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I13" s="12" t="s">
+      <c r="I13" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="5"/>
+      <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="H14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="9" t="s">
+      <c r="I14" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="J14" s="5"/>
+      <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="7" t="s">
+      <c r="H15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I15" s="9" t="s">
+      <c r="I15" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="J15" s="5"/>
+      <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H16" s="7" t="s">
+      <c r="H16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="9" t="s">
+      <c r="I16" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J16" s="5"/>
+      <c r="J16" s="2"/>
     </row>
     <row r="17" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G17" s="8"/>
-      <c r="H17" s="10" t="s">
+      <c r="G17" s="5"/>
+      <c r="H17" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="I17" s="11"/>
-      <c r="J17" s="5"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="2"/>
+    </row>
+    <row r="19" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G19" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="29">
+        <f>SUMIF(B2:B100,G20, E2:E100)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G21" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" s="29">
+        <f>SUMIF(B1:B99,G21, E1:E99)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G22" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H22" s="29">
+        <f>SUMIF(B2:B100,G22, E2:E100)</f>
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="23" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G23" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H23" s="29">
+        <f>SUMIF(B3:B101,G23, E3:E101)</f>
+        <v>3083</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E2" xr:uid="{5AAE77B6-366C-4730-A58A-C0C13BE3675F}"/>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{804FFBA0-8CD6-41DB-BA4E-0137961AF33E}">
       <formula1>$G$14:$G$16</formula1>
@@ -1380,8 +1656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D50BE8B2-990A-4D87-83F2-E814EEC1B90B}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1394,126 +1670,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="18" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="22">
+      <c r="A3" s="19">
         <f ca="1">TODAY()-30</f>
         <v>45139</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="23">
+      <c r="C3" s="21">
         <v>10000</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="23"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="22">
+      <c r="A4" s="19">
         <f ca="1">TODAY()-30</f>
         <v>45139</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="23">
+      <c r="C4" s="21">
         <v>3015</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19" t="s">
+      <c r="D4" s="22"/>
+      <c r="E4" s="23" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="22">
+      <c r="A5" s="19">
         <f ca="1">TODAY()-30</f>
         <v>45139</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="23">
+      <c r="C5" s="21">
         <v>7800</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="23" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="22">
+      <c r="A6" s="19">
         <f t="shared" ref="A6:A7" ca="1" si="0">TODAY()-30</f>
         <v>45139</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="22">
+      <c r="A7" s="19">
         <f t="shared" ca="1" si="0"/>
         <v>45139</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
+      <c r="C7" s="21">
+        <v>6352.68</v>
+      </c>
+      <c r="D7" s="22"/>
+      <c r="E7" s="23"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="22">
+      <c r="A8" s="19">
         <f ca="1">TODAY()-25</f>
         <v>45144</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="23"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="17">
+      <c r="B9" s="25"/>
+      <c r="C9" s="26">
         <f>SUBTOTAL(109,Despesas34[Valor])</f>
-        <v>20815</v>
-      </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
+        <v>27167.68</v>
+      </c>
+      <c r="D9" s="27"/>
+      <c r="E9" s="28"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">

</xml_diff>

<commit_message>
alteração colunas de atividades
</commit_message>
<xml_diff>
--- a/despesas.xlsx
+++ b/despesas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camilat2003_00\Desktop\Pessoais\Europa 06-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9CD92A-FA90-492C-94BA-2756B540CA03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1246C097-30BD-45EA-8F84-FBAB58B0A22D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -709,27 +709,27 @@
     <xf numFmtId="7" fontId="0" fillId="0" borderId="6" xfId="12" applyFont="1" applyBorder="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="6" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="7" fontId="0" fillId="0" borderId="6" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="18">
@@ -1523,67 +1523,67 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G13" s="27" t="s">
+      <c r="G13" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="27" t="s">
+      <c r="H13" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="I13" s="27" t="s">
+      <c r="I13" s="26" t="s">
         <v>20</v>
       </c>
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G14" s="28" t="s">
+      <c r="G14" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="29" t="s">
+      <c r="H14" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="28" t="s">
+      <c r="I14" s="27" t="s">
         <v>21</v>
       </c>
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G15" s="28" t="s">
+      <c r="G15" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="29" t="s">
+      <c r="H15" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="I15" s="28" t="s">
+      <c r="I15" s="27" t="s">
         <v>22</v>
       </c>
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G16" s="28" t="s">
+      <c r="G16" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="28" t="s">
+      <c r="I16" s="27" t="s">
         <v>23</v>
       </c>
       <c r="J16" s="2"/>
     </row>
     <row r="17" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="G17" s="28"/>
-      <c r="H17" s="29" t="s">
+      <c r="G17" s="27"/>
+      <c r="H17" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="I17" s="28"/>
+      <c r="I17" s="27"/>
       <c r="J17" s="2"/>
     </row>
     <row r="18" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="G18" s="30"/>
-      <c r="H18" s="29" t="s">
+      <c r="G18" s="29"/>
+      <c r="H18" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="I18" s="30"/>
+      <c r="I18" s="29"/>
       <c r="J18" s="2"/>
     </row>
     <row r="20" spans="6:10" x14ac:dyDescent="0.25">
@@ -1631,8 +1631,8 @@
       </c>
     </row>
     <row r="25" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F25" s="26"/>
-      <c r="G25" s="25" t="s">
+      <c r="F25" s="25"/>
+      <c r="G25" s="24" t="s">
         <v>35</v>
       </c>
       <c r="H25" s="23">
@@ -1662,7 +1662,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1675,13 +1675,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">

</xml_diff>